<commit_message>
truck factor calculator added
</commit_message>
<xml_diff>
--- a/Comiters/929178101.xlsx
+++ b/Comiters/929178101.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>android.view.ViewGroup; java.util.List; android.view.View; com.cjj.MaterialRefreshLayout; com.cjj.MaterialRefreshListener; android.support.v7.widget.DefaultItemAnimator; android.content.Intent; android.view.LayoutInflater; android.widget.ImageView; android.support.v7.widget.RecyclerView; android.view.MenuItem; android.os.Bundle; android.widget.ListView; java.util.Random; android.view.Menu; android.graphics.Color; android.support.v7.widget.Toolbar; android.support.annotation.Nullable; android.support.v7.widget.LinearLayoutManager; java.util.ArrayList; android.content.Context; android.widget.Toast</t>
+          <t>android.view.View; android.os.Bundle; android.widget.ImageView; android.widget.ListView; android.view.ViewGroup; com.cjj.MaterialRefreshListener; android.support.v7.widget.LinearLayoutManager; android.view.MenuItem; android.graphics.Color; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; android.support.v7.widget.Toolbar; java.util.Random; android.view.Menu; android.support.v7.widget.DefaultItemAnimator; android.support.v7.widget.RecyclerView; android.widget.Toast; java.util.List; java.util.ArrayList; android.content.Context; android.content.Intent; android.support.annotation.Nullable</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>android.view.animation.LinearInterpolator; android.view.View; android.graphics.Color; android.animation.ObjectAnimator; android.widget.FrameLayout; android.content.Context; android.util.AttributeSet; android.support.v4.view.ViewCompat; android.animation.ValueAnimator</t>
+          <t>android.animation.ValueAnimator; android.view.View; android.view.animation.LinearInterpolator; android.animation.ObjectAnimator; android.graphics.Color; android.util.AttributeSet; android.support.v4.view.ViewCompat; android.widget.FrameLayout; android.content.Context</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -484,7 +484,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>android.widget.ArrayAdapter; android.graphics.DrawFilter; android.view.ViewGroup; java.util.List; android.view.animation.LinearInterpolator; android.view.View; android.view.MotionEvent; android.graphics.RadialGradient; android.graphics.drawable.Drawable; android.graphics.drawable.shapes.OvalShape; android.support.v4.view.ViewPropertyAnimatorCompat; com.cjj.header.SunLayout; android.view.animation.Interpolator; android.view.WindowManager; com.cjj.MaterialRefreshLayout; android.graphics.PaintFlagsDrawFilter; android.graphics.Shader; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.view.animation.AccelerateDecelerateInterpolator; android.graphics.Path; android.graphics.Canvas; com.cjj.MaterialRefreshListener; android.view.animation.BounceInterpolator; android.widget.AbsListView; android.widget.FrameLayout; android.graphics.PixelFormat; android.support.v7.widget.DefaultItemAnimator; android.util.Log; android.net.Uri; android.util.DisplayMetrics; android.os.Handler; android.util.AttributeSet; android.widget.LinearLayout; android.support.v7.app.AppCompatActivity; android.content.Intent; android.graphics.Paint; android.view.LayoutInflater; android.widget.ImageView; android.support.v7.widget.RecyclerView; android.animation.ObjectAnimator; android.support.v4.view.ViewCompat; android.graphics.Paint.Style; android.view.MenuItem; android.os.Bundle; com.cjj.MaterialHeadListener; android.view.animation.Animation; android.widget.ListView; android.graphics.drawable.ShapeDrawable; android.view.animation.Transformation; android.graphics.ColorFilter; java.util.Random; android.animation.ValueAnimator; android.view.Menu; android.graphics.Rect; android.content.res.TypedArray; android.graphics.Color; android.graphics.drawable.Animatable; android.support.v7.widget.Toolbar; android.view.Gravity; android.support.annotation.Nullable; android.support.v7.widget.LinearLayoutManager; java.util.ArrayList; android.util.TypedValue; android.content.Context; android.os.Build; android.graphics.RectF; android.content.res.Resources; android.view.animation.DecelerateInterpolator; android.widget.Toast</t>
+          <t>android.view.View; android.view.animation.AccelerateDecelerateInterpolator; android.graphics.RadialGradient; android.graphics.Paint.Style; android.widget.AbsListView; com.cjj.header.SunLayout; android.os.Bundle; android.graphics.PixelFormat; android.widget.ImageView; android.widget.ListView; android.util.TypedValue; android.graphics.drawable.ShapeDrawable; com.cjj.MaterialRefreshListener; android.view.WindowManager; android.view.ViewGroup; android.support.v7.widget.LinearLayoutManager; android.graphics.Rect; android.os.Build; android.os.Handler; android.view.MenuItem; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.graphics.Color; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; android.support.v4.view.ViewPropertyAnimatorCompat; android.view.animation.BounceInterpolator; android.support.v7.widget.Toolbar; android.util.DisplayMetrics; java.util.Random; com.cjj.MaterialHeadListener; android.view.animation.DecelerateInterpolator; android.animation.ValueAnimator; android.view.animation.Transformation; android.view.Menu; android.util.Log; android.support.v7.widget.DefaultItemAnimator; android.view.animation.LinearInterpolator; android.graphics.ColorFilter; android.content.res.Resources; android.support.v7.widget.RecyclerView; android.net.Uri; android.widget.ArrayAdapter; android.view.animation.Interpolator; android.widget.Toast; java.util.List; java.util.ArrayList; android.content.Context; android.graphics.PaintFlagsDrawFilter; android.support.v7.app.AppCompatActivity; android.content.Intent; android.graphics.Shader; android.graphics.drawable.Drawable; android.graphics.drawable.Animatable; android.graphics.drawable.shapes.OvalShape; android.widget.LinearLayout; android.animation.ObjectAnimator; android.util.AttributeSet; android.content.res.TypedArray; android.view.Gravity; android.view.MotionEvent; android.support.v4.view.ViewCompat; android.support.annotation.Nullable; android.widget.FrameLayout; android.view.animation.Animation; android.graphics.Path; android.graphics.Paint; android.graphics.Canvas; android.graphics.DrawFilter; android.graphics.RectF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -497,7 +497,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>android.widget.Button; android.view.MotionEvent; android.view.ViewGroup; android.content.res.TypedArray; android.view.View; android.graphics.Color; android.support.v4.view.ViewPropertyAnimatorCompat; android.widget.AbsListView; android.view.Gravity; android.view.animation.DecelerateInterpolator; android.widget.FrameLayout; android.content.Context; android.os.Build; android.util.Log; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.util.AttributeSet; android.support.v4.view.ViewCompat</t>
+          <t>android.view.View; android.os.Build; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.util.Log; android.view.Gravity; android.graphics.Color; android.util.AttributeSet; android.content.res.TypedArray; android.view.MotionEvent; android.widget.AbsListView; android.support.v4.view.ViewCompat; android.widget.FrameLayout; android.support.v4.view.ViewPropertyAnimatorCompat; android.widget.Button; android.content.Context; android.view.ViewGroup; android.view.animation.DecelerateInterpolator</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -510,7 +510,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>android.widget.Button; android.view.MotionEvent; android.view.ViewGroup; java.util.List; android.view.View; android.support.v4.view.ViewPropertyAnimatorCompat; android.support.v4.view.ViewPropertyAnimatorUpdateListener; com.cjj.MaterialRefreshLayout; com.cjj.MaterialRefreshListener; android.widget.AbsListView; android.widget.FrameLayout; android.support.v7.widget.DefaultItemAnimator; android.util.Log; android.os.Handler; android.util.AttributeSet; android.view.LayoutInflater; android.widget.ImageView; android.support.v7.widget.RecyclerView; android.support.v4.view.ViewCompat; android.view.MenuItem; android.os.Bundle; com.cjj.MaterialHeadListener; java.util.Random; android.view.Menu; android.content.res.TypedArray; android.graphics.Color; android.support.v7.widget.Toolbar; android.view.Gravity; android.support.annotation.Nullable; android.support.v7.widget.LinearLayoutManager; java.util.ArrayList; android.view.animation.DecelerateInterpolator; android.content.Context; android.os.Build; android.widget.Toast</t>
+          <t>android.view.View; android.widget.AbsListView; android.os.Bundle; android.widget.ImageView; com.cjj.MaterialRefreshListener; android.view.ViewGroup; android.support.v7.widget.LinearLayoutManager; android.os.Handler; android.view.MenuItem; android.os.Build; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.graphics.Color; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; android.support.v4.view.ViewPropertyAnimatorCompat; android.support.v7.widget.Toolbar; java.util.Random; com.cjj.MaterialHeadListener; android.view.animation.DecelerateInterpolator; android.view.Menu; android.util.Log; android.support.v7.widget.DefaultItemAnimator; android.support.v7.widget.RecyclerView; android.widget.Toast; java.util.List; java.util.ArrayList; android.content.Context; android.view.Gravity; android.util.AttributeSet; android.content.res.TypedArray; android.view.MotionEvent; android.support.v4.view.ViewCompat; android.support.annotation.Nullable; android.widget.FrameLayout; android.widget.Button</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -523,7 +523,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>android.widget.ArrayAdapter; com.cjj.MaterialRefreshListener; android.os.Bundle; android.widget.ListView; com.cjj.MaterialRefreshLayout; android.os.Handler; android.widget.Toast</t>
+          <t>android.os.Handler; com.cjj.MaterialRefreshLayout; android.os.Bundle; android.widget.ArrayAdapter; android.widget.Toast; android.widget.ListView; com.cjj.MaterialRefreshListener</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -536,7 +536,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>android.widget.ArrayAdapter; android.widget.Button; android.view.MotionEvent; android.view.ViewGroup; java.util.List; android.view.View; android.support.v4.view.ViewPropertyAnimatorCompat; android.support.v4.view.ViewPropertyAnimatorUpdateListener; com.cjj.MaterialRefreshLayout; com.cjj.MaterialRefreshListener; android.widget.AbsListView; android.widget.FrameLayout; android.support.v7.widget.DefaultItemAnimator; android.util.Log; android.os.Handler; android.util.AttributeSet; android.view.LayoutInflater; android.widget.ImageView; android.support.v7.widget.RecyclerView; android.support.v4.view.ViewCompat; android.view.MenuItem; android.os.Bundle; com.cjj.MaterialHeadListener; android.widget.ListView; java.util.Random; android.view.Menu; android.content.res.TypedArray; android.graphics.Color; android.support.v7.widget.Toolbar; android.view.Gravity; android.support.annotation.Nullable; android.support.v7.widget.LinearLayoutManager; java.util.ArrayList; android.view.animation.DecelerateInterpolator; android.content.Context; android.os.Build; android.widget.Toast</t>
+          <t>android.view.View; android.widget.AbsListView; android.os.Bundle; android.widget.ImageView; android.widget.ListView; android.view.ViewGroup; com.cjj.MaterialRefreshListener; android.support.v7.widget.LinearLayoutManager; android.os.Handler; android.view.MenuItem; android.os.Build; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.graphics.Color; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; android.support.v4.view.ViewPropertyAnimatorCompat; android.support.v7.widget.Toolbar; java.util.Random; com.cjj.MaterialHeadListener; android.view.animation.DecelerateInterpolator; android.view.Menu; android.util.Log; android.support.v7.widget.DefaultItemAnimator; android.support.v7.widget.RecyclerView; android.widget.ArrayAdapter; android.widget.Toast; java.util.List; java.util.ArrayList; android.content.Context; android.view.Gravity; android.util.AttributeSet; android.content.res.TypedArray; android.view.MotionEvent; android.support.v4.view.ViewCompat; android.support.annotation.Nullable; android.widget.FrameLayout; android.widget.Button</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>android.widget.ArrayAdapter; android.widget.Button; android.view.MotionEvent; android.view.ViewGroup; java.util.List; android.view.View; android.graphics.RadialGradient; android.graphics.drawable.Drawable; android.graphics.drawable.shapes.OvalShape; android.support.v4.view.ViewPropertyAnimatorCompat; android.support.v4.view.ViewPropertyAnimatorUpdateListener; com.cjj.MaterialRefreshLayout; android.graphics.Shader; android.graphics.Canvas; com.cjj.MaterialRefreshListener; android.animation.AnimatorSet; android.widget.AbsListView; android.widget.FrameLayout; android.support.v7.widget.DefaultItemAnimator; android.net.Uri; android.util.Log; android.util.AttributeSet; android.content.Intent; android.graphics.Paint; android.view.LayoutInflater; android.widget.ImageView; android.support.v7.widget.RecyclerView; android.support.v4.view.ViewCompat; android.animation.ObjectAnimator; android.view.MenuItem; android.os.Bundle; com.cjj.MaterialHeadListener; android.view.animation.Animation; android.widget.ListView; android.graphics.drawable.ShapeDrawable; java.util.Random; android.view.Menu; android.content.res.TypedArray; android.graphics.Color; android.support.v7.widget.Toolbar; android.view.Gravity; android.support.annotation.Nullable; android.support.v7.widget.LinearLayoutManager; java.util.ArrayList; android.view.animation.DecelerateInterpolator; android.content.Context; android.os.Build; android.content.res.Resources; android.widget.Toast</t>
+          <t>android.view.View; android.graphics.RadialGradient; android.widget.AbsListView; android.animation.AnimatorSet; android.os.Bundle; android.widget.ImageView; android.widget.ListView; android.graphics.drawable.ShapeDrawable; android.view.ViewGroup; com.cjj.MaterialRefreshListener; android.support.v7.widget.LinearLayoutManager; android.view.MenuItem; android.os.Build; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.graphics.Color; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; android.support.v4.view.ViewPropertyAnimatorCompat; android.support.v7.widget.Toolbar; java.util.Random; com.cjj.MaterialHeadListener; android.view.animation.DecelerateInterpolator; android.view.Menu; android.util.Log; android.support.v7.widget.DefaultItemAnimator; android.content.res.Resources; android.support.v7.widget.RecyclerView; android.net.Uri; android.widget.ArrayAdapter; android.widget.Toast; java.util.List; java.util.ArrayList; android.content.Context; android.widget.Button; android.graphics.Shader; android.content.Intent; android.graphics.drawable.Drawable; android.graphics.drawable.shapes.OvalShape; android.view.Gravity; android.animation.ObjectAnimator; android.util.AttributeSet; android.content.res.TypedArray; android.view.MotionEvent; android.support.v4.view.ViewCompat; android.support.annotation.Nullable; android.view.animation.Animation; android.widget.FrameLayout; android.graphics.Paint; android.graphics.Canvas</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -562,7 +562,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>android.view.MotionEvent; android.view.ViewGroup; android.view.animation.LinearInterpolator; android.view.View; android.support.v4.view.ViewPropertyAnimatorCompat; android.graphics.drawable.Drawable; android.view.animation.Interpolator; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.view.animation.AccelerateDecelerateInterpolator; android.graphics.Path; android.graphics.Canvas; android.animation.AnimatorSet; android.widget.AbsListView; android.widget.FrameLayout; android.graphics.PixelFormat; android.util.Log; android.util.DisplayMetrics; android.util.AttributeSet; android.graphics.Paint; android.graphics.Paint.Style; android.animation.ObjectAnimator; android.view.animation.Animation; android.view.animation.Transformation; android.graphics.ColorFilter; android.graphics.Rect; android.content.res.TypedArray; android.graphics.Color; android.graphics.drawable.Animatable; android.view.Gravity; java.util.ArrayList; android.view.animation.DecelerateInterpolator; android.content.Context; android.graphics.RectF; android.os.Build; android.content.res.Resources; android.support.v4.view.ViewCompat</t>
+          <t>android.view.View; android.view.animation.AccelerateDecelerateInterpolator; android.graphics.Paint.Style; android.widget.AbsListView; android.animation.AnimatorSet; android.graphics.PixelFormat; android.view.ViewGroup; android.graphics.Rect; android.os.Build; android.support.v4.view.ViewPropertyAnimatorUpdateListener; android.graphics.Color; android.support.v4.view.ViewPropertyAnimatorCompat; android.util.DisplayMetrics; android.view.animation.DecelerateInterpolator; android.view.animation.Transformation; android.graphics.ColorFilter; android.util.Log; android.view.animation.LinearInterpolator; android.content.res.Resources; android.view.animation.Interpolator; java.util.ArrayList; android.content.Context; android.graphics.drawable.Drawable; android.graphics.drawable.Animatable; android.view.Gravity; android.animation.ObjectAnimator; android.util.AttributeSet; android.content.res.TypedArray; android.view.MotionEvent; android.support.v4.view.ViewCompat; android.widget.FrameLayout; android.graphics.Path; android.view.animation.Animation; android.graphics.Paint; android.graphics.Canvas; android.graphics.RectF</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -575,7 +575,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>android.widget.ArrayAdapter; android.view.MotionEvent; android.view.ViewGroup; java.util.List; android.view.View; android.widget.Toast; android.view.WindowManager; com.cjj.MaterialRefreshLayout; com.nineoldandroids.animation.AnimatorListenerAdapter; com.cjj.MaterialRefreshListener; android.widget.AbsListView; android.widget.FrameLayout; android.util.Log; android.support.v7.widget.DefaultItemAnimator; android.util.AttributeSet; android.widget.LinearLayout; com.nineoldandroids.animation.Animator; android.content.Intent; com.nineoldandroids.animation.AnimatorSet; android.view.LayoutInflater; android.widget.ImageView; android.support.v7.widget.RecyclerView; android.view.MenuItem; android.os.Bundle; com.cjj.MaterialHeadListener; android.view.animation.AccelerateInterpolator; android.widget.ListView; com.nineoldandroids.view.ViewHelper; java.util.Random; android.view.Menu; android.content.res.TypedArray; android.graphics.Color; android.view.animation.AnimationSet; com.nineoldandroids.animation.ValueAnimator; android.view.Gravity; android.support.v7.widget.Toolbar; android.support.annotation.Nullable; android.view.animation.DecelerateInterpolator; android.support.v7.widget.LinearLayoutManager; java.util.ArrayList; android.content.Context; android.os.Build; com.nineoldandroids.animation.ObjectAnimator; android.support.v4.view.ViewCompat</t>
+          <t>android.view.View; android.widget.AbsListView; android.os.Bundle; android.widget.ImageView; android.widget.ListView; android.view.WindowManager; android.view.ViewGroup; com.cjj.MaterialRefreshListener; android.support.v7.widget.LinearLayoutManager; android.os.Build; android.view.MenuItem; android.graphics.Color; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; com.nineoldandroids.animation.Animator; android.support.v7.widget.Toolbar; com.nineoldandroids.view.ViewHelper; java.util.Random; com.cjj.MaterialHeadListener; android.view.animation.DecelerateInterpolator; android.view.Menu; android.util.Log; android.support.v7.widget.DefaultItemAnimator; android.support.v7.widget.RecyclerView; android.widget.ArrayAdapter; android.widget.Toast; android.view.animation.AnimationSet; java.util.ArrayList; android.content.Context; java.util.List; android.content.Intent; com.nineoldandroids.animation.AnimatorSet; android.view.Gravity; android.widget.LinearLayout; android.util.AttributeSet; android.content.res.TypedArray; com.nineoldandroids.animation.ObjectAnimator; android.view.MotionEvent; com.nineoldandroids.animation.ValueAnimator; android.support.v4.view.ViewCompat; android.view.animation.AccelerateInterpolator; android.widget.FrameLayout; android.support.annotation.Nullable; com.nineoldandroids.animation.AnimatorListenerAdapter</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -588,7 +588,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>android.view.MotionEvent; android.view.ViewGroup; java.util.List; android.view.animation.LinearInterpolator; android.view.View; android.graphics.RadialGradient; android.graphics.drawable.Drawable; android.graphics.drawable.shapes.OvalShape; android.widget.Toast; android.view.animation.Interpolator; android.view.WindowManager; com.cjj.MaterialRefreshLayout; android.graphics.Shader; com.nineoldandroids.animation.AnimatorListenerAdapter; android.view.animation.AccelerateDecelerateInterpolator; android.graphics.Path; android.graphics.Canvas; com.cjj.MaterialRefreshListener; android.view.animation.BounceInterpolator; android.widget.AbsListView; android.widget.FrameLayout; android.graphics.PixelFormat; android.net.Uri; android.util.Log; android.util.DisplayMetrics; android.support.v7.widget.DefaultItemAnimator; android.os.Handler; android.util.AttributeSet; android.widget.LinearLayout; com.nineoldandroids.animation.Animator; android.support.v7.app.AppCompatActivity; com.nineoldandroids.animation.AnimatorSet; android.graphics.Paint; android.view.LayoutInflater; android.widget.ImageView; android.graphics.Paint.Style; android.support.v7.widget.RecyclerView; android.test.ApplicationTestCase; android.view.animation.Animation; android.view.animation.Transformation; android.view.animation.AccelerateInterpolator; android.graphics.drawable.ShapeDrawable; android.os.Bundle; android.view.MenuItem; android.graphics.ColorFilter; com.nineoldandroids.view.ViewHelper; java.lang.annotation.Retention; java.util.Random; android.app.Application; android.view.Menu; android.content.res.TypedArray; android.graphics.Rect; android.graphics.Color; android.view.animation.AnimationSet; android.support.annotation.NonNull; android.graphics.drawable.Animatable; android.view.Gravity; com.nineoldandroids.animation.ValueAnimator; android.support.v7.widget.Toolbar; java.util.ArrayList; android.view.animation.DecelerateInterpolator; android.support.annotation.Nullable; android.support.annotation.IntDef; android.content.Context; android.graphics.RectF; com.nineoldandroids.animation.ObjectAnimator; android.content.res.Resources; java.lang.annotation.RetentionPolicy; android.os.Build; android.support.v7.widget.LinearLayoutManager; android.support.v4.view.ViewCompat</t>
+          <t>android.view.View; android.view.animation.AccelerateDecelerateInterpolator; android.graphics.RadialGradient; android.graphics.Paint.Style; android.widget.AbsListView; android.graphics.PixelFormat; android.os.Bundle; android.widget.ImageView; android.graphics.drawable.ShapeDrawable; android.view.ViewGroup; android.view.WindowManager; android.support.v7.widget.LinearLayoutManager; com.cjj.MaterialRefreshListener; android.graphics.Rect; android.os.Build; android.os.Handler; android.view.MenuItem; android.graphics.Color; android.app.Application; android.view.LayoutInflater; com.cjj.MaterialRefreshLayout; com.nineoldandroids.animation.Animator; android.view.animation.BounceInterpolator; android.support.v7.widget.Toolbar; android.util.DisplayMetrics; com.nineoldandroids.view.ViewHelper; java.lang.annotation.RetentionPolicy; java.util.Random; android.support.annotation.NonNull; android.view.animation.DecelerateInterpolator; android.test.ApplicationTestCase; android.view.animation.Transformation; android.graphics.ColorFilter; android.util.Log; android.view.animation.LinearInterpolator; android.support.v7.widget.DefaultItemAnimator; android.view.Menu; android.content.res.Resources; android.net.Uri; android.support.v7.widget.RecyclerView; android.view.animation.Interpolator; android.widget.Toast; android.view.animation.AnimationSet; java.util.ArrayList; android.content.Context; java.util.List; android.graphics.drawable.Drawable; android.graphics.Shader; com.nineoldandroids.animation.AnimatorSet; android.support.v7.app.AppCompatActivity; android.graphics.drawable.Animatable; android.graphics.drawable.shapes.OvalShape; java.lang.annotation.Retention; android.view.Gravity; android.widget.LinearLayout; android.util.AttributeSet; android.content.res.TypedArray; com.nineoldandroids.animation.ObjectAnimator; android.view.MotionEvent; com.nineoldandroids.animation.ValueAnimator; android.support.v4.view.ViewCompat; android.view.animation.Animation; android.view.animation.AccelerateInterpolator; android.widget.FrameLayout; android.graphics.Path; android.graphics.Paint; android.support.annotation.IntDef; android.graphics.Canvas; android.support.annotation.Nullable; com.nineoldandroids.animation.AnimatorListenerAdapter; android.graphics.RectF</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>

</xml_diff>